<commit_message>
Dato agregados al excel
xxxx
</commit_message>
<xml_diff>
--- a/WEB_ADMIN/ExcelNuevoJugador.xlsx
+++ b/WEB_ADMIN/ExcelNuevoJugador.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxfl\documentos2\github\copa_frisa_capibaras_TC2007B\WEB_ADMIN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F0F014B-F23B-42AE-A38C-833E881EA085}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02163E22-F4A1-4D03-AA58-2A82FB2FC59B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6D686534-1E44-40F0-8E3C-97E3605D4FB1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="41">
   <si>
     <t>Username</t>
   </si>
@@ -135,6 +135,30 @@
   </si>
   <si>
     <t>yoemama</t>
+  </si>
+  <si>
+    <t>Yoe Mama</t>
+  </si>
+  <si>
+    <t>YoeMama@example.com</t>
+  </si>
+  <si>
+    <t>GoPro123</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1111 Consit SS</t>
+  </si>
+  <si>
+    <t>222-1234</t>
+  </si>
+  <si>
+    <t>Yoe</t>
+  </si>
+  <si>
+    <t>Mama</t>
+  </si>
+  <si>
+    <t>Reyes</t>
   </si>
 </sst>
 </file>
@@ -537,7 +561,7 @@
   <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -679,6 +703,42 @@
       <c r="A4" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="B4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="3">
+        <v>36560</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="L4" s="1">
+        <v>1234567890</v>
+      </c>
+      <c r="M4" s="1">
+        <v>3</v>
+      </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="D10" s="4"/>
@@ -687,6 +747,7 @@
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{760A51E3-C1D8-4979-909F-3A110363A897}"/>
     <hyperlink ref="C3" r:id="rId2" xr:uid="{DDFFAD46-F0C8-41CC-9E8A-25149CC358E2}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{97372063-09C2-4F66-8763-8D10A2773E75}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>